<commit_message>
added main menu, scripts for menu
also update documention, time table
</commit_message>
<xml_diff>
--- a/Documentation/JDB_UsesCaseScenario.xlsx
+++ b/Documentation/JDB_UsesCaseScenario.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessy.borcard\OneDrive - CPNV\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eurêka!\Eureka\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="PuzzleAléatoire" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
   <si>
     <t>Nom</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>en apuyant sur F1</t>
+  </si>
+  <si>
+    <t>le chemin d'accès est inaccessible</t>
+  </si>
+  <si>
+    <t>un message d'erreur est retourné au joueur</t>
   </si>
 </sst>
 </file>
@@ -714,8 +720,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,8 +963,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,7 +1222,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C35"/>
+      <selection sqref="A1:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,7 +1468,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection sqref="A1:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1545,9 +1551,15 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
+      <c r="A10" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
@@ -1683,8 +1695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>